<commit_message>
fix climb exele file change CL max take OFf from 1.9 to 2.2
</commit_message>
<xml_diff>
--- a/Matching Diagram/Drag Polar & Loverd.xlsx
+++ b/Matching Diagram/Drag Polar & Loverd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\figure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\Matching Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0B4A5E-4DFB-43B8-A058-41453F164EBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2035E85C-D913-450F-8CF0-37028216A578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="13245" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mediume" sheetId="1" r:id="rId1"/>
@@ -391,14 +391,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -44064,8 +44064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="I103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44855,7 +44855,7 @@
         <v>15.470242855400931</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="4"/>
+        <f>D8/$C$14</f>
         <v>1.6269045030267534E-2</v>
       </c>
       <c r="G8" s="1">
@@ -46037,14 +46037,14 @@
       </c>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
       <c r="T26">
         <f t="shared" si="8"/>
         <v>0.13645926343992473</v>
@@ -46102,10 +46102,10 @@
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
       <c r="T27">
         <f t="shared" si="8"/>
         <v>0.1538107421980637</v>
@@ -46292,13 +46292,13 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="11">
         <f>E29/F29</f>
         <v>621.0526315789474</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="T30">
         <f t="shared" si="8"/>
         <v>0.21304510071722779</v>
@@ -46356,20 +46356,20 @@
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
@@ -46391,49 +46391,49 @@
       <c r="E40" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="11">
         <f>F39/G39</f>
         <v>759.01328273244781</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
     </row>
     <row r="51" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="L51" s="12" t="s">
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="L51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
     </row>
     <row r="52" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="11"/>
+      <c r="H52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I52" s="10"/>
-      <c r="N52" s="10" t="s">
+      <c r="I52" s="11"/>
+      <c r="N52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10" t="s">
+      <c r="O52" s="11"/>
+      <c r="P52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Q52" s="10"/>
+      <c r="Q52" s="11"/>
     </row>
     <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
@@ -46503,59 +46503,59 @@
       <c r="D55" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="11">
         <f>10^(F54+G54*LOG(E54))</f>
         <v>3588.5867438252376</v>
       </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10">
+      <c r="G55" s="11"/>
+      <c r="H55" s="11">
         <f>10^(H54+I54*LOG(E54))</f>
         <v>4100.4228968950847</v>
       </c>
-      <c r="I55" s="10"/>
+      <c r="I55" s="11"/>
       <c r="L55" t="s">
         <v>24</v>
       </c>
-      <c r="N55" s="10">
+      <c r="N55" s="11">
         <f>10^(N54+O54*LOG(M54))</f>
         <v>4437.9855508266965</v>
       </c>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10">
+      <c r="O55" s="11"/>
+      <c r="P55" s="11">
         <f>10^(P54+Q54*LOG(M54))</f>
         <v>5157.236755434762</v>
       </c>
-      <c r="Q55" s="10"/>
+      <c r="Q55" s="11"/>
     </row>
     <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="11">
         <f>(F55+H55)/2</f>
         <v>3844.5048203601609</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
       <c r="L56" t="s">
         <v>25</v>
       </c>
-      <c r="N56" s="10">
+      <c r="N56" s="11">
         <f>(N55+P55)/2</f>
         <v>4797.6111531307288</v>
       </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
     </row>
     <row r="65" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H65" s="10" t="s">
+      <c r="H65" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
     </row>
     <row r="66" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H66" s="6"/>
@@ -46566,15 +46566,15 @@
       <c r="K66" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P66" s="10" t="s">
+      <c r="P66" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="10"/>
-      <c r="S66" s="10"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
     </row>
     <row r="67" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H67" s="11" t="s">
+      <c r="H67" s="12" t="s">
         <v>29</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -46596,7 +46596,7 @@
       </c>
     </row>
     <row r="68" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H68" s="11"/>
+      <c r="H68" s="12"/>
       <c r="I68" s="3" t="s">
         <v>31</v>
       </c>
@@ -46606,7 +46606,7 @@
       <c r="K68" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P68" s="11" t="s">
+      <c r="P68" s="12" t="s">
         <v>29</v>
       </c>
       <c r="Q68" s="3" t="s">
@@ -46620,7 +46620,7 @@
       </c>
     </row>
     <row r="69" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H69" s="11"/>
+      <c r="H69" s="12"/>
       <c r="I69" s="3" t="s">
         <v>32</v>
       </c>
@@ -46630,7 +46630,7 @@
       <c r="K69" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="P69" s="11"/>
+      <c r="P69" s="12"/>
       <c r="Q69" s="3" t="s">
         <v>31</v>
       </c>
@@ -46642,7 +46642,7 @@
       </c>
     </row>
     <row r="70" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H70" s="11"/>
+      <c r="H70" s="12"/>
       <c r="I70" s="3" t="s">
         <v>43</v>
       </c>
@@ -46652,7 +46652,7 @@
       <c r="K70" s="2">
         <v>0.02</v>
       </c>
-      <c r="P70" s="11"/>
+      <c r="P70" s="12"/>
       <c r="Q70" s="3" t="s">
         <v>32</v>
       </c>
@@ -46664,10 +46664,10 @@
       </c>
     </row>
     <row r="71" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P71" s="11"/>
+      <c r="P71" s="12"/>
       <c r="Q71" s="3" t="s">
         <v>33</v>
       </c>
@@ -46679,24 +46679,24 @@
       </c>
     </row>
     <row r="72" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H72" s="11"/>
-      <c r="P72" s="11" t="s">
+      <c r="H72" s="12"/>
+      <c r="P72" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H73" s="11"/>
+      <c r="H73" s="12"/>
       <c r="J73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="K73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="P73" s="11"/>
+      <c r="P73" s="12"/>
     </row>
     <row r="74" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H74" s="11"/>
-      <c r="P74" s="11"/>
+      <c r="H74" s="12"/>
+      <c r="P74" s="12"/>
       <c r="R74" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -46705,15 +46705,15 @@
       </c>
     </row>
     <row r="75" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="P75" s="11"/>
+      <c r="P75" s="12"/>
     </row>
     <row r="83" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I83" s="10" t="s">
+      <c r="I83" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
     </row>
     <row r="84" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I84" s="6"/>
@@ -46726,7 +46726,7 @@
       </c>
     </row>
     <row r="85" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I85" s="11" t="s">
+      <c r="I85" s="12" t="s">
         <v>29</v>
       </c>
       <c r="J85" s="3" t="s">
@@ -46740,7 +46740,7 @@
       </c>
     </row>
     <row r="86" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I86" s="11"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="3" t="s">
         <v>31</v>
       </c>
@@ -46752,7 +46752,7 @@
       </c>
     </row>
     <row r="87" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I87" s="11"/>
+      <c r="I87" s="12"/>
       <c r="J87" s="3" t="s">
         <v>32</v>
       </c>
@@ -46764,7 +46764,7 @@
       </c>
     </row>
     <row r="88" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I88" s="11"/>
+      <c r="I88" s="12"/>
       <c r="J88" s="3" t="s">
         <v>33</v>
       </c>
@@ -46776,15 +46776,15 @@
       </c>
     </row>
     <row r="89" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I89" s="11" t="s">
+      <c r="I89" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="90" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I90" s="11"/>
+      <c r="I90" s="12"/>
     </row>
     <row r="91" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I91" s="11"/>
+      <c r="I91" s="12"/>
       <c r="K91" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -46793,10 +46793,29 @@
       </c>
     </row>
     <row r="92" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I92" s="11"/>
+      <c r="I92" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I85:I88"/>
+    <mergeCell ref="I89:I92"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="P66:S66"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="P68:P71"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="P72:P75"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="P55:Q55"/>
     <mergeCell ref="L51:Q51"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="F27:G27"/>
@@ -46809,25 +46828,6 @@
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="D51:I51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I85:I88"/>
-    <mergeCell ref="I89:I92"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="P66:S66"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="P68:P71"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="P72:P75"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -48872,14 +48872,14 @@
       </c>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
       <c r="O26">
         <f t="shared" si="16"/>
         <v>6.1876946412431869E-2</v>
@@ -48944,10 +48944,10 @@
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
       <c r="O27">
         <f t="shared" si="16"/>
         <v>6.6567828945666679E-2</v>
@@ -49155,13 +49155,13 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="11">
         <f>E29/F29</f>
         <v>621.0526315789474</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="O30">
         <f t="shared" si="16"/>
         <v>8.8681989459487923E-2</v>
@@ -49271,14 +49271,14 @@
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
       <c r="O36">
         <f t="shared" si="16"/>
         <v>0.16909711860065613</v>
@@ -49288,10 +49288,10 @@
       </c>
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
       <c r="O37">
         <f t="shared" si="16"/>
         <v>0.18719052265741892</v>
@@ -49334,13 +49334,13 @@
       <c r="E40" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="11">
         <f>F39/G39</f>
         <v>759.01328273244781</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
       <c r="O40">
         <f t="shared" si="16"/>
         <v>0.24951224774182426</v>
@@ -49359,40 +49359,40 @@
       </c>
     </row>
     <row r="51" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="L51" s="12" t="s">
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="L51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
     </row>
     <row r="52" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="11"/>
+      <c r="H52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I52" s="10"/>
-      <c r="N52" s="10" t="s">
+      <c r="I52" s="11"/>
+      <c r="N52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10" t="s">
+      <c r="O52" s="11"/>
+      <c r="P52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Q52" s="10"/>
+      <c r="Q52" s="11"/>
     </row>
     <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
@@ -49462,59 +49462,59 @@
       <c r="D55" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="11">
         <f>10^(F54+G54*LOG(E54))</f>
         <v>3588.5867438252376</v>
       </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10">
+      <c r="G55" s="11"/>
+      <c r="H55" s="11">
         <f>10^(H54+I54*LOG(E54))</f>
         <v>4100.4228968950847</v>
       </c>
-      <c r="I55" s="10"/>
+      <c r="I55" s="11"/>
       <c r="L55" t="s">
         <v>24</v>
       </c>
-      <c r="N55" s="10">
+      <c r="N55" s="11">
         <f>10^(N54+O54*LOG(M54))</f>
         <v>4437.9855508266965</v>
       </c>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10">
+      <c r="O55" s="11"/>
+      <c r="P55" s="11">
         <f>10^(P54+Q54*LOG(M54))</f>
         <v>5157.236755434762</v>
       </c>
-      <c r="Q55" s="10"/>
+      <c r="Q55" s="11"/>
     </row>
     <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="11">
         <f>(F55+H55)/2</f>
         <v>3844.5048203601609</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
       <c r="L56" t="s">
         <v>25</v>
       </c>
-      <c r="N56" s="10">
+      <c r="N56" s="11">
         <f>(N55+P55)/2</f>
         <v>4797.6111531307288</v>
       </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
     </row>
     <row r="65" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H65" s="10" t="s">
+      <c r="H65" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
     </row>
     <row r="66" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H66" s="7"/>
@@ -49525,15 +49525,15 @@
       <c r="K66" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P66" s="10" t="s">
+      <c r="P66" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="10"/>
-      <c r="S66" s="10"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
     </row>
     <row r="67" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H67" s="11" t="s">
+      <c r="H67" s="12" t="s">
         <v>29</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -49555,7 +49555,7 @@
       </c>
     </row>
     <row r="68" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H68" s="11"/>
+      <c r="H68" s="12"/>
       <c r="I68" s="3" t="s">
         <v>31</v>
       </c>
@@ -49565,7 +49565,7 @@
       <c r="K68" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P68" s="11" t="s">
+      <c r="P68" s="12" t="s">
         <v>29</v>
       </c>
       <c r="Q68" s="3" t="s">
@@ -49579,7 +49579,7 @@
       </c>
     </row>
     <row r="69" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H69" s="11"/>
+      <c r="H69" s="12"/>
       <c r="I69" s="3" t="s">
         <v>32</v>
       </c>
@@ -49589,7 +49589,7 @@
       <c r="K69" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="P69" s="11"/>
+      <c r="P69" s="12"/>
       <c r="Q69" s="3" t="s">
         <v>31</v>
       </c>
@@ -49601,7 +49601,7 @@
       </c>
     </row>
     <row r="70" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H70" s="11"/>
+      <c r="H70" s="12"/>
       <c r="I70" s="3" t="s">
         <v>43</v>
       </c>
@@ -49611,7 +49611,7 @@
       <c r="K70" s="2">
         <v>0.02</v>
       </c>
-      <c r="P70" s="11"/>
+      <c r="P70" s="12"/>
       <c r="Q70" s="3" t="s">
         <v>32</v>
       </c>
@@ -49623,10 +49623,10 @@
       </c>
     </row>
     <row r="71" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P71" s="11"/>
+      <c r="P71" s="12"/>
       <c r="Q71" s="3" t="s">
         <v>33</v>
       </c>
@@ -49638,24 +49638,24 @@
       </c>
     </row>
     <row r="72" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H72" s="11"/>
-      <c r="P72" s="11" t="s">
+      <c r="H72" s="12"/>
+      <c r="P72" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H73" s="11"/>
+      <c r="H73" s="12"/>
       <c r="J73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="K73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="P73" s="11"/>
+      <c r="P73" s="12"/>
     </row>
     <row r="74" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H74" s="11"/>
-      <c r="P74" s="11"/>
+      <c r="H74" s="12"/>
+      <c r="P74" s="12"/>
       <c r="R74" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -49664,15 +49664,15 @@
       </c>
     </row>
     <row r="75" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="P75" s="11"/>
+      <c r="P75" s="12"/>
     </row>
     <row r="83" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I83" s="10" t="s">
+      <c r="I83" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
     </row>
     <row r="84" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I84" s="7"/>
@@ -49685,7 +49685,7 @@
       </c>
     </row>
     <row r="85" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I85" s="11" t="s">
+      <c r="I85" s="12" t="s">
         <v>29</v>
       </c>
       <c r="J85" s="3" t="s">
@@ -49699,7 +49699,7 @@
       </c>
     </row>
     <row r="86" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I86" s="11"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="3" t="s">
         <v>31</v>
       </c>
@@ -49711,7 +49711,7 @@
       </c>
     </row>
     <row r="87" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I87" s="11"/>
+      <c r="I87" s="12"/>
       <c r="J87" s="3" t="s">
         <v>32</v>
       </c>
@@ -49723,7 +49723,7 @@
       </c>
     </row>
     <row r="88" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I88" s="11"/>
+      <c r="I88" s="12"/>
       <c r="J88" s="3" t="s">
         <v>33</v>
       </c>
@@ -49735,15 +49735,15 @@
       </c>
     </row>
     <row r="89" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I89" s="11" t="s">
+      <c r="I89" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="90" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I90" s="11"/>
+      <c r="I90" s="12"/>
     </row>
     <row r="91" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I91" s="11"/>
+      <c r="I91" s="12"/>
       <c r="K91" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -49752,10 +49752,29 @@
       </c>
     </row>
     <row r="92" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I92" s="11"/>
+      <c r="I92" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I85:I88"/>
+    <mergeCell ref="I89:I92"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="P66:S66"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="P68:P71"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="P72:P75"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="P55:Q55"/>
     <mergeCell ref="L51:Q51"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="F27:G27"/>
@@ -49768,25 +49787,6 @@
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="D51:I51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I85:I88"/>
-    <mergeCell ref="I89:I92"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="P66:S66"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="P68:P71"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="P72:P75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -51770,14 +51770,14 @@
       </c>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
       <c r="T26">
         <f t="shared" si="4"/>
         <v>0.12362868748099662</v>
@@ -51835,10 +51835,10 @@
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
       <c r="T27">
         <f t="shared" si="4"/>
         <v>0.14009788765821327</v>
@@ -52025,13 +52025,13 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="11">
         <f>E29/F29</f>
         <v>621.0526315789474</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="T30">
         <f t="shared" si="4"/>
         <v>0.19632032964250459</v>
@@ -52089,20 +52089,20 @@
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
@@ -52124,49 +52124,49 @@
       <c r="E40" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="11">
         <f>F39/G39</f>
         <v>759.01328273244781</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
     </row>
     <row r="51" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="L51" s="12" t="s">
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="L51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
     </row>
     <row r="52" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="11"/>
+      <c r="H52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I52" s="10"/>
-      <c r="N52" s="10" t="s">
+      <c r="I52" s="11"/>
+      <c r="N52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10" t="s">
+      <c r="O52" s="11"/>
+      <c r="P52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Q52" s="10"/>
+      <c r="Q52" s="11"/>
     </row>
     <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
@@ -52236,59 +52236,59 @@
       <c r="D55" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="11">
         <f>10^(F54+G54*LOG(E54))</f>
         <v>3588.5867438252376</v>
       </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10">
+      <c r="G55" s="11"/>
+      <c r="H55" s="11">
         <f>10^(H54+I54*LOG(E54))</f>
         <v>4100.4228968950847</v>
       </c>
-      <c r="I55" s="10"/>
+      <c r="I55" s="11"/>
       <c r="L55" t="s">
         <v>24</v>
       </c>
-      <c r="N55" s="10">
+      <c r="N55" s="11">
         <f>10^(N54+O54*LOG(M54))</f>
         <v>4437.9855508266965</v>
       </c>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10">
+      <c r="O55" s="11"/>
+      <c r="P55" s="11">
         <f>10^(P54+Q54*LOG(M54))</f>
         <v>5157.236755434762</v>
       </c>
-      <c r="Q55" s="10"/>
+      <c r="Q55" s="11"/>
     </row>
     <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="11">
         <f>(F55+H55)/2</f>
         <v>3844.5048203601609</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
       <c r="L56" t="s">
         <v>25</v>
       </c>
-      <c r="N56" s="10">
+      <c r="N56" s="11">
         <f>(N55+P55)/2</f>
         <v>4797.6111531307288</v>
       </c>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
     </row>
     <row r="65" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H65" s="10" t="s">
+      <c r="H65" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
     </row>
     <row r="66" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H66" s="7"/>
@@ -52299,15 +52299,15 @@
       <c r="K66" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P66" s="10" t="s">
+      <c r="P66" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="10"/>
-      <c r="S66" s="10"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
     </row>
     <row r="67" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H67" s="11" t="s">
+      <c r="H67" s="12" t="s">
         <v>29</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -52329,7 +52329,7 @@
       </c>
     </row>
     <row r="68" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H68" s="11"/>
+      <c r="H68" s="12"/>
       <c r="I68" s="3" t="s">
         <v>31</v>
       </c>
@@ -52339,7 +52339,7 @@
       <c r="K68" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P68" s="11" t="s">
+      <c r="P68" s="12" t="s">
         <v>29</v>
       </c>
       <c r="Q68" s="3" t="s">
@@ -52353,7 +52353,7 @@
       </c>
     </row>
     <row r="69" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H69" s="11"/>
+      <c r="H69" s="12"/>
       <c r="I69" s="3" t="s">
         <v>32</v>
       </c>
@@ -52363,7 +52363,7 @@
       <c r="K69" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="P69" s="11"/>
+      <c r="P69" s="12"/>
       <c r="Q69" s="3" t="s">
         <v>31</v>
       </c>
@@ -52375,7 +52375,7 @@
       </c>
     </row>
     <row r="70" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H70" s="11"/>
+      <c r="H70" s="12"/>
       <c r="I70" s="3" t="s">
         <v>43</v>
       </c>
@@ -52385,7 +52385,7 @@
       <c r="K70" s="2">
         <v>0.02</v>
       </c>
-      <c r="P70" s="11"/>
+      <c r="P70" s="12"/>
       <c r="Q70" s="3" t="s">
         <v>32</v>
       </c>
@@ -52397,10 +52397,10 @@
       </c>
     </row>
     <row r="71" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P71" s="11"/>
+      <c r="P71" s="12"/>
       <c r="Q71" s="3" t="s">
         <v>33</v>
       </c>
@@ -52412,24 +52412,24 @@
       </c>
     </row>
     <row r="72" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H72" s="11"/>
-      <c r="P72" s="11" t="s">
+      <c r="H72" s="12"/>
+      <c r="P72" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H73" s="11"/>
+      <c r="H73" s="12"/>
       <c r="J73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="K73" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="P73" s="11"/>
+      <c r="P73" s="12"/>
     </row>
     <row r="74" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H74" s="11"/>
-      <c r="P74" s="11"/>
+      <c r="H74" s="12"/>
+      <c r="P74" s="12"/>
       <c r="R74" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -52438,15 +52438,15 @@
       </c>
     </row>
     <row r="75" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="P75" s="11"/>
+      <c r="P75" s="12"/>
     </row>
     <row r="83" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I83" s="10" t="s">
+      <c r="I83" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
     </row>
     <row r="84" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I84" s="7"/>
@@ -52459,7 +52459,7 @@
       </c>
     </row>
     <row r="85" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I85" s="11" t="s">
+      <c r="I85" s="12" t="s">
         <v>29</v>
       </c>
       <c r="J85" s="3" t="s">
@@ -52473,7 +52473,7 @@
       </c>
     </row>
     <row r="86" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I86" s="11"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="3" t="s">
         <v>31</v>
       </c>
@@ -52485,7 +52485,7 @@
       </c>
     </row>
     <row r="87" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I87" s="11"/>
+      <c r="I87" s="12"/>
       <c r="J87" s="3" t="s">
         <v>32</v>
       </c>
@@ -52497,7 +52497,7 @@
       </c>
     </row>
     <row r="88" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I88" s="11"/>
+      <c r="I88" s="12"/>
       <c r="J88" s="3" t="s">
         <v>33</v>
       </c>
@@ -52509,15 +52509,15 @@
       </c>
     </row>
     <row r="89" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I89" s="11" t="s">
+      <c r="I89" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="90" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I90" s="11"/>
+      <c r="I90" s="12"/>
     </row>
     <row r="91" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I91" s="11"/>
+      <c r="I91" s="12"/>
       <c r="K91" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -52526,10 +52526,29 @@
       </c>
     </row>
     <row r="92" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I92" s="11"/>
+      <c r="I92" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I85:I88"/>
+    <mergeCell ref="I89:I92"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="P66:S66"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="P68:P71"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="P72:P75"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="P55:Q55"/>
     <mergeCell ref="L51:Q51"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="F27:G27"/>
@@ -52542,25 +52561,6 @@
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="D51:I51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I85:I88"/>
-    <mergeCell ref="I89:I92"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="P66:S66"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="P68:P71"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="P72:P75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>